<commit_message>
fix Num of Cluster(100 data)
</commit_message>
<xml_diff>
--- a/excel/Machinery_Part/Section1.xlsx
+++ b/excel/Machinery_Part/Section1.xlsx
@@ -26290,7 +26290,7 @@
       </c>
       <c r="BD36" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>(+)25 &amp; (+)% &amp; (+),70 &amp; (+)% &amp; (+)△1 &amp; (-)1/2 &amp; (-)3/4</t>
         </is>
       </c>
       <c r="BE36" t="inlineStr">
@@ -28585,7 +28585,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:CX12"/>
+  <dimension ref="A1:CX13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -34760,6 +34760,519 @@
         </is>
       </c>
     </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>, exhaust gas back pressure of 6.0 kPa at 100% load
+△2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="M13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="O13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="P13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Q13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="R13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="S13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="T13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="U13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="V13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="W13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="X13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Y13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="Z13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AA13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AB13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AC13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AD13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AE13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AF13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AG13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AH13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AI13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AJ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AK13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AL13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AM13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AN13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AO13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AP13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AQ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AR13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AS13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AT13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AU13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AV13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AW13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AX13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AY13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="AZ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BA13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BB13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BC13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BD13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BE13" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="BF13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BG13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BH13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BI13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BJ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BK13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BL13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BM13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BN13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BO13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BP13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BQ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BR13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BS13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BT13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BU13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BV13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BW13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BX13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BY13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="BZ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CA13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CB13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CC13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CD13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CE13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CF13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CG13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CH13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CI13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CJ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CK13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CL13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CM13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CN13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CO13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CP13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CQ13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CR13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CS13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CT13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CU13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CV13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CW13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="CX13" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>

</xml_diff>